<commit_message>
Created data tables for each different event type
</commit_message>
<xml_diff>
--- a/data/BMHC_MarCom_Impact_Report.xlsx
+++ b/data/BMHC_MarCom_Impact_Report.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CxLos\OneDrive\Documents\BMHC\2024\Monthly Reports\November\MC_Impact_11_2024\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6433551F-528D-4CE9-BFD8-01FE993FCA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="BMHC Monthly Report - MarCom" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Sheet1" sheetId="3" r:id="rId6"/>
+    <sheet name="Responses" sheetId="1" r:id="rId1"/>
+    <sheet name="MarCom" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Timestamp</t>
   </si>
@@ -157,17 +166,6 @@
     <t>Health Awareness &amp; Education Acitivity</t>
   </si>
   <si>
-    <t>BMHC MarCom Report - October 2024</t>
-  </si>
-  <si>
-    <t>MarCom 
-Reporting Month</t>
-  </si>
-  <si>
-    <t>BMHC Organizational 
-Communications/Marketing Activities</t>
-  </si>
-  <si>
     <t>BMHC Organizational
 Public Information</t>
   </si>
@@ -280,50 +278,73 @@
 * Blacks Have the Highest Risk for Colorectal Cancer (10/4); 
 </t>
   </si>
+  <si>
+    <t>MarCom
+Reporting Month</t>
+  </si>
+  <si>
+    <t>BMHC Organizational
+Communications/Marketing Activities</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="13">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF442F65"/>
@@ -337,6 +358,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -351,6 +373,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -365,6 +388,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -379,6 +403,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -393,6 +418,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -407,6 +433,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -421,6 +448,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -435,6 +463,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -449,6 +478,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -463,6 +493,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -477,6 +508,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -491,210 +523,265 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf quotePrefix="1" borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font/>
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b/>
+      </font>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F9FA"/>
+          <bgColor rgb="FFF8F9FA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF5B3F86"/>
           <bgColor rgb="FF5B3F86"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F9FA"/>
+          <bgColor rgb="FFF8F9FA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFFFF"/>
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF8F9FA"/>
-          <bgColor rgb="FFF8F9FA"/>
+          <fgColor rgb="FF5B3F86"/>
+          <bgColor rgb="FF5B3F86"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle count="3" pivot="0" name="Form Responses 1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Form Responses 1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="firstRowStripe" dxfId="24"/>
+      <tableStyleElement type="secondRowStripe" dxfId="23"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="BMHC Monthly Report - MarCom-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="BMHC Monthly Report - MarCom-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+      <tableStyleElement type="headerRow" dxfId="22"/>
+      <tableStyleElement type="firstRowStripe" dxfId="21"/>
+      <tableStyleElement type="secondRowStripe" dxfId="20"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:R3" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:R3">
   <tableColumns count="18">
-    <tableColumn name="Timestamp" id="1"/>
-    <tableColumn name="Which report are you submitting? (Month and Year)" id="2"/>
-    <tableColumn name="Organizational Communications/Marketing" id="3"/>
-    <tableColumn name="Organizational Public Information" id="4"/>
-    <tableColumn name="Organizational Products" id="5"/>
-    <tableColumn name="Organizational Event-Oriented" id="6"/>
-    <tableColumn name="Care Network Communications/Marketing" id="7"/>
-    <tableColumn name="Care Network  Public Information" id="8"/>
-    <tableColumn name="Care Network  Products" id="9"/>
-    <tableColumn name="Care Network Event-Oriented" id="10"/>
-    <tableColumn name="Know Your Numbers Communications/Marketing" id="11"/>
-    <tableColumn name="Know Your Numbers Public Information" id="12"/>
-    <tableColumn name="Know Your Numbers Products" id="13"/>
-    <tableColumn name="Know Your Numbers Event Oriented:" id="14"/>
-    <tableColumn name="Health Awareness &amp; ED Communications/Marketing" id="15"/>
-    <tableColumn name="Health Awareness &amp; ED Public Information" id="16"/>
-    <tableColumn name="Health Awareness &amp; ED Products" id="17"/>
-    <tableColumn name="Health Awareness &amp; ED Event-Oriented" id="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Timestamp"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Which report are you submitting? (Month and Year)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Organizational Communications/Marketing"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Organizational Public Information"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Organizational Products"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Organizational Event-Oriented"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Care Network Communications/Marketing"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Care Network  Public Information"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Care Network  Products"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Care Network Event-Oriented"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Know Your Numbers Communications/Marketing"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Know Your Numbers Public Information"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Know Your Numbers Products"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Know Your Numbers Event Oriented:"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Health Awareness &amp; ED Communications/Marketing"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Health Awareness &amp; ED Public Information"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Health Awareness &amp; ED Products"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Health Awareness &amp; ED Event-Oriented"/>
   </tableColumns>
-  <tableStyleInfo name="Form Responses 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Form Responses 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:Q4" displayName="Form_Responses1_2" name="Form_Responses1_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Form_Responses1_2" displayName="Form_Responses1_2" ref="A1:Q3" headerRowDxfId="0" dataDxfId="1" totalsRowDxfId="2">
   <tableColumns count="17">
-    <tableColumn name="MarCom _x000a_Reporting Month" id="1"/>
-    <tableColumn name="BMHC Organizational _x000a_Communications/Marketing Activities" id="2"/>
-    <tableColumn name="BMHC Organizational_x000a_Public Information" id="3"/>
-    <tableColumn name="BMHC Organizational _x000a_Products" id="4"/>
-    <tableColumn name="BMHC Organizational_x000a_Event-Oriented" id="5"/>
-    <tableColumn name="Care Network Enhancement_x000a_Communications/Marketing" id="6"/>
-    <tableColumn name="Care Network Enhancement_x000a_Public Information" id="7"/>
-    <tableColumn name="Care Network Enhancement_x000a_Products" id="8"/>
-    <tableColumn name="Care Network Enhancement_x000a_Event-Oriented" id="9"/>
-    <tableColumn name="Know Your Numbers_x000a_Communications/Marketing" id="10"/>
-    <tableColumn name="Know Your Numbers_x000a_Public Information" id="11"/>
-    <tableColumn name="Know Your Numbers_x000a_Products" id="12"/>
-    <tableColumn name="Know Your Numbers_x000a_Event Oriented" id="13"/>
-    <tableColumn name="Health Awareness &amp; ED_x000a_Communications/Marketing" id="14"/>
-    <tableColumn name="Health Awareness &amp; ED_x000a_Public Information" id="15"/>
-    <tableColumn name="Health Awareness &amp; ED_x000a_Products" id="16"/>
-    <tableColumn name="Health Awareness &amp; ED_x000a_Event-Oriented" id="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="MarCom_x000a_Reporting Month" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="BMHC Organizational_x000a_Communications/Marketing Activities" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="BMHC Organizational_x000a_Public Information" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="BMHC Organizational _x000a_Products" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BMHC Organizational_x000a_Event-Oriented" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Care Network Enhancement_x000a_Communications/Marketing" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Care Network Enhancement_x000a_Public Information" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Care Network Enhancement_x000a_Products" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Care Network Enhancement_x000a_Event-Oriented" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Know Your Numbers_x000a_Communications/Marketing" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Know Your Numbers_x000a_Public Information" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Know Your Numbers_x000a_Products" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Know Your Numbers_x000a_Event Oriented" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Health Awareness &amp; ED_x000a_Communications/Marketing" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Health Awareness &amp; ED_x000a_Public Information" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Health Awareness &amp; ED_x000a_Products" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Health Awareness &amp; ED_x000a_Event-Oriented" dataDxfId="3"/>
   </tableColumns>
-  <tableStyleInfo name="BMHC Monthly Report - MarCom-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="BMHC Monthly Report - MarCom-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -884,44 +971,47 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.88"/>
-    <col customWidth="1" min="2" max="2" width="37.63"/>
-    <col customWidth="1" min="3" max="3" width="36.5"/>
-    <col customWidth="1" min="4" max="4" width="29.63"/>
-    <col customWidth="1" min="5" max="5" width="35.63"/>
-    <col customWidth="1" min="6" max="6" width="26.88"/>
-    <col customWidth="1" min="7" max="7" width="35.88"/>
-    <col customWidth="1" min="8" max="8" width="29.38"/>
-    <col customWidth="1" min="9" max="9" width="22.63"/>
-    <col customWidth="1" min="10" max="10" width="26.25"/>
-    <col customWidth="1" min="11" max="11" width="37.63"/>
-    <col customWidth="1" min="12" max="12" width="33.88"/>
-    <col customWidth="1" min="13" max="13" width="27.13"/>
-    <col customWidth="1" min="14" max="14" width="31.5"/>
-    <col customWidth="1" min="15" max="15" width="37.63"/>
-    <col customWidth="1" min="16" max="16" width="36.0"/>
-    <col customWidth="1" min="17" max="17" width="29.25"/>
-    <col customWidth="1" min="18" max="18" width="33.25"/>
-    <col customWidth="1" min="19" max="24" width="18.88"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="35.88671875" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.21875" customWidth="1"/>
+    <col min="11" max="11" width="37.6640625" customWidth="1"/>
+    <col min="12" max="12" width="33.88671875" customWidth="1"/>
+    <col min="13" max="13" width="27.109375" customWidth="1"/>
+    <col min="14" max="14" width="31.44140625" customWidth="1"/>
+    <col min="15" max="15" width="37.6640625" customWidth="1"/>
+    <col min="16" max="16" width="36" customWidth="1"/>
+    <col min="17" max="17" width="29.21875" customWidth="1"/>
+    <col min="18" max="18" width="33.21875" customWidth="1"/>
+    <col min="19" max="24" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,9 +1067,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>45603.71747101852</v>
+        <v>45603.717471018521</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -1005,7 +1095,7 @@
       <c r="I2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
@@ -1015,7 +1105,7 @@
       <c r="M2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="7"/>
+      <c r="N2" s="6"/>
       <c r="O2" s="6" t="s">
         <v>29</v>
       </c>
@@ -1025,223 +1115,217 @@
       <c r="Q2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="9">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>45607.548570960644</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="12"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="10"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B4" sqref="B4" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.88"/>
-    <col customWidth="1" min="2" max="2" width="37.63"/>
-    <col customWidth="1" min="3" max="3" width="36.5"/>
-    <col customWidth="1" min="4" max="4" width="29.63"/>
-    <col customWidth="1" min="5" max="5" width="22.75"/>
-    <col customWidth="1" min="6" max="6" width="26.88"/>
-    <col customWidth="1" min="7" max="7" width="28.13"/>
-    <col customWidth="1" min="8" max="8" width="28.88"/>
-    <col customWidth="1" min="9" max="9" width="26.38"/>
-    <col customWidth="1" min="10" max="10" width="26.25"/>
-    <col customWidth="1" min="11" max="11" width="25.13"/>
-    <col customWidth="1" min="12" max="12" width="20.75"/>
-    <col customWidth="1" min="13" max="13" width="19.88"/>
-    <col customWidth="1" min="14" max="14" width="25.63"/>
-    <col customWidth="1" min="15" max="15" width="31.0"/>
-    <col customWidth="1" min="16" max="16" width="27.88"/>
-    <col customWidth="1" min="17" max="17" width="24.63"/>
-    <col customWidth="1" min="18" max="18" width="33.25"/>
-    <col customWidth="1" min="19" max="24" width="18.88"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" customWidth="1"/>
+    <col min="10" max="10" width="26.21875" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" customWidth="1"/>
+    <col min="12" max="12" width="20.77734375" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" customWidth="1"/>
+    <col min="15" max="15" width="31" customWidth="1"/>
+    <col min="16" max="16" width="27.88671875" customWidth="1"/>
+    <col min="17" max="17" width="24.6640625" customWidth="1"/>
+    <col min="18" max="18" width="33.21875" customWidth="1"/>
+    <col min="19" max="24" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:17" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>34</v>
       </c>
+      <c r="D1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="15" t="s">
+    <row r="2" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+    </row>
+    <row r="3" spans="1:17" ht="399" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="C3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="E3" s="11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="20"/>
-    </row>
-    <row r="4" ht="399.0" customHeight="1">
-      <c r="A4" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="22" t="s">
+      <c r="F3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="G3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="23"/>
-      <c r="N4" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" s="22" t="s">
+      <c r="P3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q3" s="12" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
-  </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>